<commit_message>
add integration tests for the new config mode
</commit_message>
<xml_diff>
--- a/data/blueprints/library/test/quickfort/list/all_modes_separate_sheets.xlsx
+++ b/data/blueprints/library/test/quickfort/list/all_modes_separate_sheets.xlsx
@@ -8,10 +8,11 @@
     <sheet state="visible" name="place_sheet" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="zone_sheet" sheetId="4" r:id="rId7"/>
     <sheet state="visible" name="query_sheet" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="meta_sheet" sheetId="6" r:id="rId9"/>
-    <sheet state="visible" name="notes_sheet" sheetId="7" r:id="rId10"/>
-    <sheet state="visible" name="ignore_sheet" sheetId="8" r:id="rId11"/>
-    <sheet state="visible" name="aliases_sheet" sheetId="9" r:id="rId12"/>
+    <sheet state="visible" name="config_sheet" sheetId="6" r:id="rId9"/>
+    <sheet state="visible" name="meta_sheet" sheetId="7" r:id="rId10"/>
+    <sheet state="visible" name="notes_sheet" sheetId="8" r:id="rId11"/>
+    <sheet state="visible" name="ignore_sheet" sheetId="9" r:id="rId12"/>
+    <sheet state="visible" name="aliases_sheet" sheetId="10" r:id="rId13"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>#dig hidden()</t>
   </si>
@@ -34,6 +35,9 @@
   </si>
   <si>
     <t>#query hidden()</t>
+  </si>
+  <si>
+    <t>#config hidden()</t>
   </si>
   <si>
     <t>#meta hidden()</t>
@@ -52,16 +56,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
-    <font/>
     <font>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -78,14 +83,11 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -97,6 +99,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -334,7 +340,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -346,6 +352,26 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
@@ -354,7 +380,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -374,7 +400,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -394,7 +420,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -414,7 +440,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -434,7 +460,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -454,7 +480,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -474,10 +500,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="s">
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -494,10 +520,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="s">
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
reorder sheets to be more useful
put aliases and ignore in the middle to test blueprint ordering
</commit_message>
<xml_diff>
--- a/data/blueprints/library/test/quickfort/list/all_modes_separate_sheets.xlsx
+++ b/data/blueprints/library/test/quickfort/list/all_modes_separate_sheets.xlsx
@@ -9,10 +9,10 @@
     <sheet state="visible" name="zone_sheet" sheetId="4" r:id="rId7"/>
     <sheet state="visible" name="query_sheet" sheetId="5" r:id="rId8"/>
     <sheet state="visible" name="config_sheet" sheetId="6" r:id="rId9"/>
-    <sheet state="visible" name="meta_sheet" sheetId="7" r:id="rId10"/>
-    <sheet state="visible" name="notes_sheet" sheetId="8" r:id="rId11"/>
-    <sheet state="visible" name="ignore_sheet" sheetId="9" r:id="rId12"/>
-    <sheet state="visible" name="aliases_sheet" sheetId="10" r:id="rId13"/>
+    <sheet state="visible" name="ignore_sheet" sheetId="7" r:id="rId10"/>
+    <sheet state="visible" name="aliases_sheet" sheetId="8" r:id="rId11"/>
+    <sheet state="visible" name="meta_sheet" sheetId="9" r:id="rId12"/>
+    <sheet state="visible" name="notes_sheet" sheetId="10" r:id="rId13"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -40,16 +40,16 @@
     <t>#config hidden()</t>
   </si>
   <si>
+    <t>#ignore</t>
+  </si>
+  <si>
+    <t>#aliases</t>
+  </si>
+  <si>
     <t>#meta hidden()</t>
   </si>
   <si>
     <t>#notes hidden()</t>
-  </si>
-  <si>
-    <t>#ignore</t>
-  </si>
-  <si>
-    <t>#aliases</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
[quickfort] add documentation and test data for config mode (#2070)
- documents the new config mode
- adds integration test data for [quickfort] implement config mode scripts#361
- adds a note recommending that config mode be used instead of the quickfort query_unsafe setting
- converts the dreamfort /setup blueprint to use config mode; also adjust the aliases used in that blueprint to no longer escape from and re-enter query mode
- adds some more distinctive anchor names for the quickfort and blueprint guides
</commit_message>
<xml_diff>
--- a/data/blueprints/library/test/quickfort/list/all_modes_separate_sheets.xlsx
+++ b/data/blueprints/library/test/quickfort/list/all_modes_separate_sheets.xlsx
@@ -8,10 +8,11 @@
     <sheet state="visible" name="place_sheet" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="zone_sheet" sheetId="4" r:id="rId7"/>
     <sheet state="visible" name="query_sheet" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="meta_sheet" sheetId="6" r:id="rId9"/>
-    <sheet state="visible" name="notes_sheet" sheetId="7" r:id="rId10"/>
-    <sheet state="visible" name="ignore_sheet" sheetId="8" r:id="rId11"/>
-    <sheet state="visible" name="aliases_sheet" sheetId="9" r:id="rId12"/>
+    <sheet state="visible" name="config_sheet" sheetId="6" r:id="rId9"/>
+    <sheet state="visible" name="ignore_sheet" sheetId="7" r:id="rId10"/>
+    <sheet state="visible" name="aliases_sheet" sheetId="8" r:id="rId11"/>
+    <sheet state="visible" name="meta_sheet" sheetId="9" r:id="rId12"/>
+    <sheet state="visible" name="notes_sheet" sheetId="10" r:id="rId13"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>#dig hidden()</t>
   </si>
@@ -36,32 +37,36 @@
     <t>#query hidden()</t>
   </si>
   <si>
+    <t>#config hidden()</t>
+  </si>
+  <si>
+    <t>#ignore</t>
+  </si>
+  <si>
+    <t>#aliases</t>
+  </si>
+  <si>
     <t>#meta hidden()</t>
   </si>
   <si>
     <t>#notes hidden()</t>
-  </si>
-  <si>
-    <t>#ignore</t>
-  </si>
-  <si>
-    <t>#aliases</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
-    <font/>
     <font>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -78,14 +83,11 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -97,6 +99,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -334,7 +340,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -346,6 +352,26 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
@@ -354,7 +380,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -374,7 +400,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -394,7 +420,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -414,7 +440,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -434,7 +460,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -454,7 +480,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -474,10 +500,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="s">
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -494,10 +520,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="s">
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>